<commit_message>
Updated the issue report
</commit_message>
<xml_diff>
--- a/Issues/BubbleChess_Issue_Report.xlsx
+++ b/Issues/BubbleChess_Issue_Report.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16420"/>
   </bookViews>
   <sheets>
     <sheet name="issueExport" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="67">
   <si>
     <t>Summary</t>
   </si>
@@ -76,7 +81,8 @@
     <t>validAttack() returns true for squares in front of a pawn</t>
   </si>
   <si>
-    <t>The pawn can move to occupy the squares ahead of it, but the pawn does not threaten those squares._x000D__x000D__x000D__x000D_Change validAttack() so it recognizes this case and returns false.</t>
+    <t>The pawn can move to occupy the squares ahead of it, but the pawn does not threaten those squares.
+Change validAttack() so it recognizes this case and returns false.</t>
   </si>
   <si>
     <t>CheckForMove invalid parameters</t>
@@ -100,13 +106,19 @@
     <t>Store games</t>
   </si>
   <si>
-    <t>Store games in db_x000D__x000D__x000D__x000D_GameId_x000D__x000D_userId1 (white)_x000D__x000D_userId2 (black)_x000D__x000D_GameOver</t>
+    <t>Store games in db
+GameId
+userId1 (white)
+userId2 (black)
+GameOver</t>
   </si>
   <si>
     <t>Check Login Update</t>
   </si>
   <si>
-    <t>Success and user ID_x000D__x000D_Password incorrect result="incorrect password"_x000D__x000D_User not found 'user not found'</t>
+    <t>Success and user ID
+Password incorrect result="incorrect password"
+User not found 'user not found'</t>
   </si>
   <si>
     <t>createUser update</t>
@@ -136,25 +148,56 @@
     <t>Return a result for checkLogin</t>
   </si>
   <si>
-    <t>result': 'success' and the 'userID' for correct info_x000D__x000D_'result':'incorrect password'_x000D__x000D_'result':'user' not found' for invalid username</t>
+    <t>result': 'success' and the 'userID' for correct info
+'result':'incorrect password'
+'result':'user' not found' for invalid username</t>
   </si>
   <si>
     <t>Call to updateState() in applyMove() creates infinite loop</t>
   </si>
   <si>
-    <t>The call to updateState() at the end of applyMove() (line 156) creates an infinite, recursive loop._x000D__x000D__x000D__x000D_updateState() -&gt; hasValidMove() -&gt; getMoves() -&gt; validMove() -&gt; applyMoveCloning() -&gt; applyMove() -&gt; updateState()_x000D__x000D__x000D__x000D_When updating the state, hasValidMove is called to make sure the position is not in an end-state such as stalemate or checkmate. This means that we have to generate moves for the opponent, and check to see if at least one is legal. The problem occurs when we find a legal move and apply it to the board, because applyMove will update the state again. This is unnecessary and should be circumvented - once validMove returns true, we are done._x000D__x000D_</t>
+    <t xml:space="preserve">The call to updateState() at the end of applyMove() (line 156) creates an infinite, recursive loop.
+updateState() -&gt; hasValidMove() -&gt; getMoves() -&gt; validMove() -&gt; applyMoveCloning() -&gt; applyMove() -&gt; updateState()
+When updating the state, hasValidMove is called to make sure the position is not in an end-state such as stalemate or checkmate. This means that we have to generate moves for the opponent, and check to see if at least one is legal. The problem occurs when we find a legal move and apply it to the board, because applyMove will update the state again. This is unnecessary and should be circumvented - once validMove returns true, we are done.
+</t>
   </si>
   <si>
     <t>Returning captured pieces in ChessBoard creates impossible downcast</t>
   </si>
   <si>
-    <t>On line 84 of ChessBoard.java, there is a bug when trying to cast an arraylist to an array.  Explination is in the following FindBugs report:_x000D__x000D__x000D__x000D_Bug: Impossible downcast of toArray() result to com.bubblechess.client.BoardPiece[] in com.bubblechess.client.ChessBoard.getCaptured()_x000D__x000D__x000D__x000D_This code is casting the result of calling toArray() on a collection to a type more specific than Object[], as in:_x000D__x000D_```_x000D__x000D_String[] getAsArray(Collection&lt;String&gt; c) {_x000D__x000D_  return (String[]) c.toArray();_x000D__x000D_  }_x000D__x000D_```_x000D__x000D__x000D__x000D__x000D__x000D_This will usually fail by throwing a ClassCastException. The toArray() of almost all collections return an Object[]. They can't really do anything else, since the Collection object has no reference to the declared generic type of the collection. _x000D__x000D__x000D__x000D_The correct way to do get an array of a specific type from a collection is to use c.toArray(new String[]); or c.toArray(new String[c.size()]); (the latter is slightly more efficient). _x000D__x000D__x000D__x000D_There is one common/known exception exception to this. The toArray() method of lists returned by Arrays.asList(...) will return a covariantly typed array. For example, Arrays.asArray(new String[] { "a" }).toArray() will return a String []. FindBugs attempts to detect and suppress such cases, but may miss some. _x000D__x000D__x000D__x000D_Rank: Scary (5), confidence: High_x000D__x000D_Pattern: BC_IMPOSSIBLE_DOWNCAST_OF_TOARRAY _x000D__x000D_Type: BC, Category: CORRECTNESS (Correctness)_x000D__x000D_</t>
+    <t xml:space="preserve">On line 84 of ChessBoard.java, there is a bug when trying to cast an arraylist to an array.  Explination is in the following FindBugs report:
+Bug: Impossible downcast of toArray() result to com.bubblechess.client.BoardPiece[] in com.bubblechess.client.ChessBoard.getCaptured()
+This code is casting the result of calling toArray() on a collection to a type more specific than Object[], as in:
+```
+String[] getAsArray(Collection&lt;String&gt; c) {
+  return (String[]) c.toArray();
+  }
+```
+This will usually fail by throwing a ClassCastException. The toArray() of almost all collections return an Object[]. They can't really do anything else, since the Collection object has no reference to the declared generic type of the collection. 
+The correct way to do get an array of a specific type from a collection is to use c.toArray(new String[]); or c.toArray(new String[c.size()]); (the latter is slightly more efficient). 
+There is one common/known exception exception to this. The toArray() method of lists returned by Arrays.asList(...) will return a covariantly typed array. For example, Arrays.asArray(new String[] { "a" }).toArray() will return a String []. FindBugs attempts to detect and suppress such cases, but may miss some. 
+Rank: Scary (5), confidence: High
+Pattern: BC_IMPOSSIBLE_DOWNCAST_OF_TOARRAY 
+Type: BC, Category: CORRECTNESS (Correctness)
+</t>
   </si>
   <si>
     <t>Implemented Board Pieces mask field in superclass (ChessPiece)</t>
   </si>
   <si>
-    <t>Severity: Low priority_x000D__x000D__x000D__x000D_In the implementation of each BoardPiece, the overridden directional vector (`dirs`) masks the vector created in the superclass.  These values should be set in the constructor, not the class body._x000D__x000D__x000D__x000D_Before (Queen.java):_x000D__x000D_```java_x000D__x000D_protected int[][] dirs = {N,NE,E,SE,S,SW,W,NW};_x000D__x000D_```_x000D__x000D__x000D__x000D_After (Queen.java):_x000D__x000D_```java_x000D__x000D_public Queen(Color col) {_x000D__x000D_	color = col;_x000D__x000D_	dirs = new int[][]{N,NE,E,SE,S,SW,W,NW};_x000D__x000D_}_x000D__x000D_```</t>
+    <t>Severity: Low priority
+In the implementation of each BoardPiece, the overridden directional vector (`dirs`) masks the vector created in the superclass.  These values should be set in the constructor, not the class body.
+Before (Queen.java):
+```java
+protected int[][] dirs = {N,NE,E,SE,S,SW,W,NW};
+```
+After (Queen.java):
+```java
+public Queen(Color col) {
+	color = col;
+	dirs = new int[][]{N,NE,E,SE,S,SW,W,NW};
+}
+```</t>
   </si>
   <si>
     <t>When two users are playing a game they should be notified when an endstate is reached</t>
@@ -184,7 +227,8 @@
     <t>Continue as guest option</t>
   </si>
   <si>
-    <t>This will essentially just create a user with a random username (generate a random 10 char username)_x000D__x000D_Return result success and userID</t>
+    <t>This will essentially just create a user with a random username (generate a random 10 char username)
+Return result success and userID</t>
   </si>
   <si>
     <t>Severity</t>
@@ -197,13 +241,31 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>Game Crash if no joinable games</t>
+  </si>
+  <si>
+    <t>The game crashes is there is nothing in the list of joinable games and you try to join</t>
+  </si>
+  <si>
+    <t>Game does not refresh the board until opponent move</t>
+  </si>
+  <si>
+    <t>The game does not refresh the board until the opponent has made his move</t>
+  </si>
+  <si>
+    <t>Please also check the github issues page below</t>
+  </si>
+  <si>
+    <t>https://github.com/markkohdev/BubbleChess/issues</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1027,23 +1089,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="76.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45">
+    <row r="2" spans="1:9" ht="28">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1089,7 +1152,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:9" ht="28">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1111,8 +1174,11 @@
       <c r="G3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="45">
+      <c r="I3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1134,8 +1200,11 @@
       <c r="G4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30">
+      <c r="I4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1158,7 +1227,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="60">
+    <row r="6" spans="1:9" ht="98">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1181,7 +1250,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45">
+    <row r="7" spans="1:9" ht="42">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1204,7 +1273,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30">
+    <row r="8" spans="1:9" ht="28">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1227,7 +1296,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1247,7 +1316,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30">
+    <row r="10" spans="1:9" ht="154">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1270,7 +1339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45">
+    <row r="11" spans="1:9" ht="70">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1293,7 +1362,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1316,7 +1385,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1339,7 +1408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="60">
+    <row r="14" spans="1:9" ht="42">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1362,7 +1431,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1385,7 +1454,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45">
+    <row r="16" spans="1:9" ht="70">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1408,7 +1477,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="240">
+    <row r="17" spans="1:7" ht="308">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1431,7 +1500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="360">
+    <row r="18" spans="1:7" ht="409">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -1454,7 +1523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="150">
+    <row r="19" spans="1:7" ht="409">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -1477,7 +1546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="60">
+    <row r="20" spans="1:7" ht="56">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -1500,7 +1569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="90">
+    <row r="21" spans="1:7" ht="70">
       <c r="A21" s="1" t="s">
         <v>51</v>
       </c>
@@ -1523,7 +1592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="60">
+    <row r="22" spans="1:7" ht="56">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
@@ -1546,7 +1615,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45">
+    <row r="23" spans="1:7" ht="56">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -1569,8 +1638,59 @@
         <v>25</v>
       </c>
     </row>
+    <row r="24" spans="1:7" ht="28">
+      <c r="A24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="28">
+      <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed gui refresh and join game issues
from the issue report and known issues section sin the release notes
</commit_message>
<xml_diff>
--- a/Issues/BubbleChess_Issue_Report.xlsx
+++ b/Issues/BubbleChess_Issue_Report.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16420"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="issueExport" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="63">
   <si>
     <t>Summary</t>
   </si>
@@ -243,18 +243,6 @@
     <t>Low</t>
   </si>
   <si>
-    <t>Game Crash if no joinable games</t>
-  </si>
-  <si>
-    <t>The game crashes is there is nothing in the list of joinable games and you try to join</t>
-  </si>
-  <si>
-    <t>Game does not refresh the board until opponent move</t>
-  </si>
-  <si>
-    <t>The game does not refresh the board until the opponent has made his move</t>
-  </si>
-  <si>
     <t>Please also check the github issues page below</t>
   </si>
   <si>
@@ -264,8 +252,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1089,21 +1077,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="76.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1129,7 +1117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28">
+    <row r="2" spans="1:9" ht="45">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1152,7 +1140,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28">
+    <row r="3" spans="1:9" ht="45">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1175,10 +1163,10 @@
         <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="28">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1201,10 +1189,10 @@
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="28">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1227,7 +1215,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="98">
+    <row r="6" spans="1:9" ht="120">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1250,7 +1238,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="42">
+    <row r="7" spans="1:9" ht="45">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1273,7 +1261,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="28">
+    <row r="8" spans="1:9" ht="30">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1316,7 +1304,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="154">
+    <row r="10" spans="1:9" ht="165">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1339,7 +1327,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="70">
+    <row r="11" spans="1:9" ht="75">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1385,7 +1373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="30">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1408,7 +1396,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="42">
+    <row r="14" spans="1:9" ht="60">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1431,7 +1419,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="30">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1454,7 +1442,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="70">
+    <row r="16" spans="1:9" ht="75">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1477,7 +1465,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="308">
+    <row r="17" spans="1:7" ht="360">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1500,7 +1488,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="409">
+    <row r="18" spans="1:7" ht="409.5">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -1523,7 +1511,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="409">
+    <row r="19" spans="1:7" ht="409.5">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -1546,7 +1534,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="56">
+    <row r="20" spans="1:7" ht="60">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -1569,7 +1557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="70">
+    <row r="21" spans="1:7" ht="90">
       <c r="A21" s="1" t="s">
         <v>51</v>
       </c>
@@ -1592,7 +1580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="56">
+    <row r="22" spans="1:7" ht="60">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
@@ -1615,7 +1603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="56">
+    <row r="23" spans="1:7" ht="75">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -1635,52 +1623,6 @@
         <v>50</v>
       </c>
       <c r="G23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="28">
-      <c r="A24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="28">
-      <c r="A25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>